<commit_message>
more informations to final report
</commit_message>
<xml_diff>
--- a/diretorio_entrega_final/Pre_Relatorio_Template.xlsx
+++ b/diretorio_entrega_final/Pre_Relatorio_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\mql_python\diretorio_entrega_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFE8462-C975-4F0D-BAD4-9D27A27D132E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59ED44A6-8B35-4462-9205-D3DDBDBF92FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{396ECD6C-DF2C-430C-8957-7F8082EF8F41}"/>
   </bookViews>
@@ -66,34 +66,34 @@
     <t>Qual Plataforma Testou a estratégia</t>
   </si>
   <si>
-    <t xml:space="preserve">Ay Senninha Long Only </t>
-  </si>
-  <si>
-    <t>Homenagem ao Ayrton Senna, relacionando seu bom resultado com uma boa direção para as operações</t>
-  </si>
-  <si>
-    <t>Quando uma ação está sobrecomprada consideramos que há uma maior chance de haver uma correção em seu preço.</t>
-  </si>
-  <si>
     <t>Trade</t>
   </si>
   <si>
     <t xml:space="preserve">Ações </t>
   </si>
   <si>
-    <t xml:space="preserve">Ações do Ibovespa </t>
-  </si>
-  <si>
     <t xml:space="preserve">Python </t>
   </si>
   <si>
     <t>Superar o Ibovespa</t>
   </si>
   <si>
-    <t>121 operações</t>
-  </si>
-  <si>
     <t>1,73 dias em média</t>
+  </si>
+  <si>
+    <t>81 operações</t>
+  </si>
+  <si>
+    <t>Ações do Ibovespa 02/2016</t>
+  </si>
+  <si>
+    <t>Existem pares de ações que tem suas variações relacionadas de alguma forma, exemplo: “no passado, quando o ativo A subia X%, o ativo B subia Y%”. Com isso, quando é observado que houve uma variação que não condiz com esse padrão, é aberta uma operação acreditando que essa relação voltará ao normal.</t>
+  </si>
+  <si>
+    <t>Ay Senninha Long &amp; Short</t>
+  </si>
+  <si>
+    <t>Homenagem ao Ayrton Senna, relacionando seu bom resultado com uma boa direção para as operações. 'Ay' além da iniciais do nome, é um trocadilho com 'AI' de artificial intelligence.</t>
   </si>
 </sst>
 </file>
@@ -288,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -320,6 +320,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4699ACC1-D5E8-4129-B413-2E96A2750F28}">
   <dimension ref="B1:C18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,28 +846,28 @@
       <c r="B8" s="10"/>
       <c r="C8" s="13"/>
     </row>
-    <row r="9" spans="2:3" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="2:3" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="84.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="123" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="137.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -872,7 +875,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -880,7 +883,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -888,7 +891,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -896,7 +899,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -904,7 +907,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -912,7 +915,7 @@
         <v>9</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -920,7 +923,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>